<commit_message>
Automatische test-sync: 2025-09-02 22:58:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-09-02.xlsx
+++ b/logs/mail_log_2025-09-02.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2</f>
+              <f>'Dashboard'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2</f>
+              <f>'Dashboard'!$B$2:$B$3</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -725,8 +725,50 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Bestelling M6 bouten</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>"Testbedrijf 123 B.V." &lt;klantenservice@testbedrijf123.nl&gt;</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-09-02 22:57:55</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="D2:D3">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -746,7 +788,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
+  <conditionalFormatting sqref="G2:G3">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -754,17 +796,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="H2:H3">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="I2:I3">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2">
+  <conditionalFormatting sqref="J2:J3">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -779,7 +821,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -809,6 +851,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-09-02 23:08:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-09-02.xlsx
+++ b/logs/mail_log_2025-09-02.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -767,8 +767,50 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Bestelling M6 bouten</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>"Testbedrijf 123 B.V." &lt;planning@testbedrijf123.nl&gt;</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Inkoop / Bestellingen</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-09-02 23:08:13</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D4">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -788,7 +830,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
+  <conditionalFormatting sqref="G2:G4">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -796,17 +838,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3">
+  <conditionalFormatting sqref="H2:H4">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I3">
+  <conditionalFormatting sqref="I2:I4">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J3">
+  <conditionalFormatting sqref="J2:J4">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -844,17 +886,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Inkoop / Bestellingen</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Inkoop / Bestellingen</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B3" t="n">

</xml_diff>